<commit_message>
Update Diccionario de variables.xlsx
</commit_message>
<xml_diff>
--- a/stores/Diccionario de variables.xlsx
+++ b/stores/Diccionario de variables.xlsx
@@ -8,30 +8,31 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes-my.sharepoint.com/personal/af_diaz27_uniandes_edu_co/Documents/Maestría en Economía Aplicada/Big Data y Machine Learning/Taller 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="489" documentId="8_{B3BAE68F-C3B3-4D0C-8927-44A6A46D73DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{667D5557-2E65-4922-8508-57D130AD19E9}"/>
+  <xr:revisionPtr revIDLastSave="522" documentId="8_{B3BAE68F-C3B3-4D0C-8927-44A6A46D73DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{51C3636F-EB8D-41A3-9164-BAD0E73D269C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="766" firstSheet="1" activeTab="1" xr2:uid="{9746C94E-B379-42DB-9985-B4ADFAF467BC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="766" firstSheet="1" activeTab="3" xr2:uid="{9746C94E-B379-42DB-9985-B4ADFAF467BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja11" sheetId="15" state="hidden" r:id="rId1"/>
     <sheet name="Hogar" sheetId="1" r:id="rId2"/>
     <sheet name="Individuo" sheetId="3" r:id="rId3"/>
-    <sheet name="VariablesIndTrain" sheetId="9" state="hidden" r:id="rId4"/>
-    <sheet name="VariablesIndTest" sheetId="10" state="hidden" r:id="rId5"/>
-    <sheet name="RenameIndTrain" sheetId="12" state="hidden" r:id="rId6"/>
-    <sheet name="RenameIndTest" sheetId="14" state="hidden" r:id="rId7"/>
-    <sheet name="VariablesHogarTrain" sheetId="4" state="hidden" r:id="rId8"/>
-    <sheet name="VariablesHogarTest" sheetId="6" state="hidden" r:id="rId9"/>
-    <sheet name="RenameHogarTrain" sheetId="7" state="hidden" r:id="rId10"/>
-    <sheet name="RenameHogarTest" sheetId="8" state="hidden" r:id="rId11"/>
+    <sheet name="Propuesta de variables nuevas" sheetId="16" r:id="rId4"/>
+    <sheet name="VariablesIndTrain" sheetId="9" state="hidden" r:id="rId5"/>
+    <sheet name="VariablesIndTest" sheetId="10" state="hidden" r:id="rId6"/>
+    <sheet name="RenameIndTrain" sheetId="12" state="hidden" r:id="rId7"/>
+    <sheet name="RenameIndTest" sheetId="14" state="hidden" r:id="rId8"/>
+    <sheet name="VariablesHogarTrain" sheetId="4" state="hidden" r:id="rId9"/>
+    <sheet name="VariablesHogarTest" sheetId="6" state="hidden" r:id="rId10"/>
+    <sheet name="RenameHogarTrain" sheetId="7" state="hidden" r:id="rId11"/>
+    <sheet name="RenameHogarTest" sheetId="8" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Hogar!$A$1:$G$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Individuo!$A$1:$I$137</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">RenameHogarTest!$A$1:$C$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">RenameHogarTrain!$A$1:$C$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">RenameIndTest!$A$1:$C$7</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">RenameIndTrain!$A$1:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">RenameHogarTest!$A$1:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">RenameHogarTrain!$A$1:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">RenameIndTest!$A$1:$C$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">RenameIndTrain!$A$1:$C$7</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1530" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1546" uniqueCount="621">
   <si>
     <t>id</t>
   </si>
@@ -1979,6 +1980,54 @@
   </si>
   <si>
     <t>'Sexo', 'JefeHogar', 'FormalSalud', 'SeguridadSocial', 'maxEducLevel', 'relab', 'SubsAlimen', 'SubsTrans', 'SubsFamil', 'SubsEducativo', 'Viaticos', 'Bonificaciones', 'FormalPension', 'MasHoras', 'PagosExtraPensArri', 'Ayuda', 'GanancFinan', 'EdadTrabajo', 'Ocu', 'Desocu', 'Inact'</t>
+  </si>
+  <si>
+    <t>¿Es la jefe de hogar mujer?</t>
+  </si>
+  <si>
+    <t>Edad de la jefe de hogar</t>
+  </si>
+  <si>
+    <t>Educación de la jefe de hogar</t>
+  </si>
+  <si>
+    <t>relab de la jefe de hogar</t>
+  </si>
+  <si>
+    <t>porcentaje de los que trabajan reciben subsidios</t>
+  </si>
+  <si>
+    <t>porcentaje de los que trabajan reciben bonificaciones y viáticos</t>
+  </si>
+  <si>
+    <t>Porcentaje de los que tienen una educación universitaria</t>
+  </si>
+  <si>
+    <t>Porcentaje de los que trabajan cotizan en salud</t>
+  </si>
+  <si>
+    <t>Porcentaje de los que trabajan cotizan en pensión</t>
+  </si>
+  <si>
+    <t>Al menos uno recibe PagosExtraPensArri</t>
+  </si>
+  <si>
+    <t>porcentaje de los que trabajan reciben Ayuda</t>
+  </si>
+  <si>
+    <t>porcentaje de los que trabajan reciben GanancFinan</t>
+  </si>
+  <si>
+    <t>Porcentaje de Edad Trabajo</t>
+  </si>
+  <si>
+    <t>Porcentaje de Ocu cuando Edad Trabajo = 1</t>
+  </si>
+  <si>
+    <t>Porcentaje de Desocu cuando Edad Trabajo = 1</t>
+  </si>
+  <si>
+    <t>Porcentaje de Inact cuando Edad Trabajo = 1</t>
   </si>
 </sst>
 </file>
@@ -2065,7 +2114,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>982980</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2127,8 +2176,8 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>622935</xdr:colOff>
-      <xdr:row>93</xdr:row>
-      <xdr:rowOff>409575</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2189,7 +2238,7 @@
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>622935</xdr:colOff>
-      <xdr:row>96</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2833,6 +2882,203 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3A793F-4067-4F02-AC6E-92BEC6450CC0}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="135" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="str">
+        <f>+"'"&amp;A2&amp;"'"</f>
+        <v>'id'</v>
+      </c>
+      <c r="C2" t="str">
+        <f>+B2</f>
+        <v>'id'</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B14" si="0">+"'"&amp;A3&amp;"'"</f>
+        <v>'Clase'</v>
+      </c>
+      <c r="C3" t="str">
+        <f>+C2&amp;", "&amp;B3</f>
+        <v>'id', 'Clase'</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>'Dominio'</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C14" si="1">+C3&amp;", "&amp;B4</f>
+        <v>'id', 'Clase', 'Dominio'</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>'P5000'</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000'</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>'P5010'</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010'</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>'P5090'</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090'</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>'P5100'</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100'</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>'P5130'</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130'</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>'P5140'</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140'</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>'Nper'</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper'</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>'Npersug'</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper', 'Npersug'</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>'Li'</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper', 'Npersug', 'Li'</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>'Lp'</v>
+      </c>
+      <c r="C14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper', 'Npersug', 'Li', 'Lp'</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>599</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D58C747-4A1F-47B8-BAE9-F1FABE2D4B92}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -2964,7 +3210,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C552F82-AAFD-4FD5-99F6-DF47FD6A8B74}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -3100,7 +3346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF217B8-2030-4600-B584-F55ACA93E4FD}">
   <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
@@ -3674,10 +3920,10 @@
   <dimension ref="A1:I137"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B134" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E140" sqref="E140"/>
+      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3722,7 +3968,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3869,7 +4115,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>214</v>
       </c>
@@ -3898,7 +4144,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>216</v>
       </c>
@@ -3927,7 +4173,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>219</v>
       </c>
@@ -3956,7 +4202,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>222</v>
       </c>
@@ -3985,7 +4231,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>225</v>
       </c>
@@ -4014,7 +4260,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>228</v>
       </c>
@@ -4147,7 +4393,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>240</v>
       </c>
@@ -4436,7 +4682,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>272</v>
       </c>
@@ -4517,7 +4763,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>280</v>
       </c>
@@ -4598,7 +4844,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>288</v>
       </c>
@@ -4679,7 +4925,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>296</v>
       </c>
@@ -5124,7 +5370,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>344</v>
       </c>
@@ -5179,7 +5425,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>349</v>
       </c>
@@ -5312,7 +5558,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>363</v>
       </c>
@@ -5341,7 +5587,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>366</v>
       </c>
@@ -5370,7 +5616,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>369</v>
       </c>
@@ -5503,7 +5749,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>383</v>
       </c>
@@ -5844,7 +6090,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>421</v>
       </c>
@@ -6159,7 +6405,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>454</v>
       </c>
@@ -6214,7 +6460,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>459</v>
       </c>
@@ -6373,7 +6619,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>474</v>
       </c>
@@ -6402,7 +6648,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>477</v>
       </c>
@@ -6431,7 +6677,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>480</v>
       </c>
@@ -6460,7 +6706,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>483</v>
       </c>
@@ -7326,11 +7572,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:I137" xr:uid="{003C75AC-219E-4BA0-819A-3C6A1AE25886}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Train"/>
-      </filters>
-    </filterColumn>
     <filterColumn colId="3">
       <filters>
         <filter val="Sí"/>
@@ -7343,6 +7584,101 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECCE2F0-11B8-451F-9201-EF8EBCC58C32}">
+  <dimension ref="B2:B17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>620</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD84958D-150B-4576-A773-2484EB5E7AF0}">
   <dimension ref="A1:C29"/>
   <sheetViews>
@@ -7708,7 +8044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABBE7710-6004-4F50-A78C-446FFA7D8F40}">
   <dimension ref="A1:C28"/>
   <sheetViews>
@@ -8061,7 +8397,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C530E332-939C-416F-BC41-7B3FB0A83185}">
   <dimension ref="A1:D28"/>
   <sheetViews>
@@ -8497,7 +8833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE11CFE-9C41-48FE-9CF8-53D4E69479EC}">
   <dimension ref="A1:D27"/>
   <sheetViews>
@@ -8917,7 +9253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06AE955D-ABF5-447B-9CD1-C698657EB110}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -9177,201 +9513,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3A793F-4067-4F02-AC6E-92BEC6450CC0}">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="135" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="str">
-        <f>+"'"&amp;A2&amp;"'"</f>
-        <v>'id'</v>
-      </c>
-      <c r="C2" t="str">
-        <f>+B2</f>
-        <v>'id'</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B14" si="0">+"'"&amp;A3&amp;"'"</f>
-        <v>'Clase'</v>
-      </c>
-      <c r="C3" t="str">
-        <f>+C2&amp;", "&amp;B3</f>
-        <v>'id', 'Clase'</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>'Dominio'</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C14" si="1">+C3&amp;", "&amp;B4</f>
-        <v>'id', 'Clase', 'Dominio'</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>'P5000'</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000'</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>'P5010'</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010'</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>'P5090'</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090'</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>'P5100'</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100'</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>'P5130'</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130'</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>'P5140'</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140'</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="str">
-        <f t="shared" si="0"/>
-        <v>'Nper'</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper'</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="str">
-        <f t="shared" si="0"/>
-        <v>'Npersug'</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper', 'Npersug'</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" si="0"/>
-        <v>'Li'</v>
-      </c>
-      <c r="C13" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper', 'Npersug', 'Li'</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="str">
-        <f t="shared" si="0"/>
-        <v>'Lp'</v>
-      </c>
-      <c r="C14" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>'id', 'Clase', 'Dominio', 'P5000', 'P5010', 'P5090', 'P5100', 'P5130', 'P5140', 'Nper', 'Npersug', 'Li', 'Lp'</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>599</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>